<commit_message>
2025-03-01 upload done from linux machine
</commit_message>
<xml_diff>
--- a/data_collection/category.xlsx
+++ b/data_collection/category.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B164"/>
+  <dimension ref="A1:B165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2401,6 +2401,18 @@
         </is>
       </c>
     </row>
+    <row r="165">
+      <c r="A165" s="1" t="inlineStr">
+        <is>
+          <t>도시락 및 식사용 조리식품 제조업</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Uncategorized</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
2025-05-03 upload done from linux machine
</commit_message>
<xml_diff>
--- a/data_collection/category.xlsx
+++ b/data_collection/category.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B165"/>
+  <dimension ref="A1:B168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2413,6 +2413,42 @@
         </is>
       </c>
     </row>
+    <row r="166">
+      <c r="A166" s="1" t="inlineStr">
+        <is>
+          <t>비거주 복지시설 운영업</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Uncategorized</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="inlineStr">
+        <is>
+          <t>자동차 차체나 트레일러 제조업</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Uncategorized</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="inlineStr">
+        <is>
+          <t>개인 및 가정용품 수리업</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Uncategorized</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>